<commit_message>
separate lung,trachea and bronchus
</commit_message>
<xml_diff>
--- a/output/HR_summary_365.xlsx
+++ b/output/HR_summary_365.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -446,12 +446,12 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>upper</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>lower</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>upper</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -489,30 +489,30 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Malignant neoplasm of trachea, bronchus and lung</t>
+          <t>Other and unspecified malignant neoplasm of skin</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1.23</v>
+        <v>1.33</v>
       </c>
       <c r="E2" t="n">
-        <v>2.1</v>
+        <v>1.08</v>
       </c>
       <c r="F2" t="n">
-        <v>1.62</v>
+        <v>1.2</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="I2" t="n">
-        <v>244</v>
+        <v>1457</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>1.62[2.1, 1.23]</t>
+          <t>1.2[1.08, 1.33]</t>
         </is>
       </c>
     </row>
@@ -525,17 +525,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Other malignant neoplasms of lymphoid and histiocytic tissue</t>
+          <t>Malignant neoplasm of trachea, bronchus and lung</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1.33</v>
+        <v>2.06</v>
       </c>
       <c r="E3" t="n">
-        <v>2.56</v>
+        <v>1.24</v>
       </c>
       <c r="F3" t="n">
-        <v>1.87</v>
+        <v>1.62</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -544,11 +544,11 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>174</v>
+        <v>244</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>1.87[2.56, 1.33]</t>
+          <t>1.62[1.24, 2.06]</t>
         </is>
       </c>
     </row>
@@ -561,17 +561,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Multiple myeloma and immunoproliferative neoplasms</t>
+          <t>Other malignant neoplasms of lymphoid and histiocytic tissue</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1.3</v>
+        <v>2.47</v>
       </c>
       <c r="E4" t="n">
-        <v>3.47</v>
+        <v>1.41</v>
       </c>
       <c r="F4" t="n">
-        <v>2.15</v>
+        <v>1.9</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -580,11 +580,11 @@
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>73</v>
+        <v>205</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>2.15[3.47, 1.3]</t>
+          <t>1.9[1.41, 2.47]</t>
         </is>
       </c>
     </row>
@@ -597,17 +597,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Lymphoid leukemia</t>
+          <t>Malignant melanoma of skin</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.99</v>
+        <v>1.41</v>
       </c>
       <c r="E5" t="n">
-        <v>3.11</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="F5" t="n">
-        <v>1.83</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -616,11 +616,11 @@
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>47</v>
+        <v>101</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>1.83[3.11, 0.99]</t>
+          <t>1.0[0.69, 1.41]</t>
         </is>
       </c>
     </row>
@@ -633,17 +633,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Myeloid leukemia</t>
+          <t>Multiple myeloma and immunoproliferative neoplasms</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1.02</v>
+        <v>3.56</v>
       </c>
       <c r="E6" t="n">
-        <v>4.06</v>
+        <v>1.26</v>
       </c>
       <c r="F6" t="n">
-        <v>2.09</v>
+        <v>2.15</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -652,11 +652,11 @@
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>2.09[4.06, 1.02]</t>
+          <t>2.15[1.26, 3.56]</t>
         </is>
       </c>
     </row>
@@ -669,17 +669,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Lymphosarcoma and reticulosarcoma</t>
+          <t>Lymphoid leukemia</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.87</v>
+        <v>3.32</v>
       </c>
       <c r="E7" t="n">
-        <v>4.07</v>
+        <v>0.97</v>
       </c>
       <c r="F7" t="n">
-        <v>2.06</v>
+        <v>1.83</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -688,11 +688,11 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>2.06[4.07, 0.87]</t>
+          <t>1.83[0.97, 3.32]</t>
         </is>
       </c>
     </row>
@@ -705,17 +705,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Hodgkin's disease</t>
+          <t>Myeloid leukemia</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.83</v>
+        <v>4.08</v>
       </c>
       <c r="E8" t="n">
-        <v>3.79</v>
+        <v>0.95</v>
       </c>
       <c r="F8" t="n">
-        <v>1.99</v>
+        <v>2.09</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -724,11 +724,11 @@
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>1.99[3.79, 0.83]</t>
+          <t>2.09[0.95, 4.08]</t>
         </is>
       </c>
     </row>
@@ -741,17 +741,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Leukemia of unspecified cell type</t>
+          <t>Hodgkin's disease</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.57</v>
+        <v>3.93</v>
       </c>
       <c r="E9" t="n">
-        <v>5.04</v>
+        <v>0.85</v>
       </c>
       <c r="F9" t="n">
-        <v>1.87</v>
+        <v>1.99</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -760,11 +760,11 @@
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>1.87[5.04, 0.57]</t>
+          <t>1.99[0.85, 3.93]</t>
         </is>
       </c>
     </row>
@@ -777,17 +777,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Malignant neoplasm of larynx</t>
+          <t>Leukemia of unspecified cell type</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.65</v>
+        <v>5.56</v>
       </c>
       <c r="E10" t="n">
-        <v>4.97</v>
+        <v>0.53</v>
       </c>
       <c r="F10" t="n">
-        <v>2.21</v>
+        <v>1.87</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
@@ -796,36 +796,34 @@
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>2.21[4.97, 0.65]</t>
+          <t>1.87[0.53, 5.56]</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B11" t="n">
         <v>365</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Malignant neoplasm of other and ill-defined sites within the respiratory system and intrathoracic organs</t>
+          <t>Malignant neoplasm of larynx</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+        <v>5.33</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.65</v>
       </c>
       <c r="F11" t="n">
-        <v>3.88</v>
+        <v>2.21</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -834,11 +832,11 @@
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>3.88[inf, 0.0]</t>
+          <t>2.21[0.65, 5.33]</t>
         </is>
       </c>
     </row>

</xml_diff>